<commit_message>
Added the voltage divider's to the battery balancing board and updated the part's list
</commit_message>
<xml_diff>
--- a/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
+++ b/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
@@ -484,7 +484,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -567,7 +567,7 @@
         <v>0.1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -596,7 +596,7 @@
         <v>0.1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added supporting components for the SHDN pin to the schematic and part's list
</commit_message>
<xml_diff>
--- a/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
+++ b/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t>100K Resistor</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT100K</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 5% 1/8W 0805</t>
   </si>
 </sst>
 </file>
@@ -114,7 +126,22 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,11 +186,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -481,142 +510,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B097BF0F-8E66-4B45-A292-B7ED4A5324CC}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="10" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="2" customWidth="1"/>
+    <col min="4" max="6" width="22.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="34.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="23.109375" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>0.1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>0.1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>0.1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -629,8 +691,11 @@
     <hyperlink ref="H4" r:id="rId5" xr:uid="{65F00B7B-66D2-4281-9659-385AA46ECFE7}"/>
     <hyperlink ref="I4" r:id="rId6" display="RMCF Series, Packaging Spec" xr:uid="{93B45437-BE8C-4FA0-90C6-E818BB7141CB}"/>
     <hyperlink ref="J4" r:id="rId7" xr:uid="{AC699323-30B6-441C-9324-25F881B7ABCC}"/>
+    <hyperlink ref="I5" r:id="rId8" display="RMCF Series, Packaging Spec" xr:uid="{7F65EBAB-61AF-4589-A1CB-D538092BA30D}"/>
+    <hyperlink ref="J5" r:id="rId9" xr:uid="{1C75C55A-B852-4291-B6D7-9037B0466635}"/>
+    <hyperlink ref="H5" r:id="rId10" xr:uid="{DA2334BA-4C4D-494B-8CEB-BDD8360C2A7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the IRF7458PbF N-Channel MOSFET SMD Footprint to eagleLibraries
</commit_message>
<xml_diff>
--- a/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
+++ b/Project QUBO/eagleDesigns/powerBoard/Powerboard Component List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Packaging Specs</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity </t>
-  </si>
-  <si>
     <t>100K Resistor</t>
   </si>
   <si>
@@ -155,7 +152,28 @@
     <t>C0G Dielectric 10-250V</t>
   </si>
   <si>
-    <t>s</t>
+    <t>Min Quantity (No Backups)</t>
+  </si>
+  <si>
+    <t>N-Channel Mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infineon Technologies </t>
+  </si>
+  <si>
+    <t>IRF7458TRPBF</t>
+  </si>
+  <si>
+    <t>IRF7458PBFCT-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 30V 14A 8-SOIC</t>
+  </si>
+  <si>
+    <t>IRF7458PbF</t>
+  </si>
+  <si>
+    <t>X7R Dielectric, 6.3-250 VDC</t>
   </si>
 </sst>
 </file>
@@ -219,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -227,12 +245,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -563,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B097BF0F-8E66-4B45-A292-B7ED4A5324CC}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,17 +609,17 @@
     <col min="7" max="7" width="23.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="40.5546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="13.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2">
         <f>SUM(D4:D20)</f>
-        <v>1.9200000000000004</v>
+        <v>16.84</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -600,11 +630,11 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
+      <c r="C3" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -672,7 +702,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D9" si="0">(B5*C5)</f>
+        <f t="shared" ref="D5:D10" si="0">(B5*C5)</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -732,29 +762,29 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3">
         <v>0.1</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>12</v>
@@ -768,70 +798,103 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3">
         <v>0.52</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>0.52</v>
+        <v>1.04</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3">
         <v>0.1</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="B10" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -848,9 +911,11 @@
     <hyperlink ref="I8" r:id="rId11" xr:uid="{E29978C5-44F3-4F96-8CDF-34370FD0D528}"/>
     <hyperlink ref="J8" r:id="rId12" display="X2Y Series Datasheet" xr:uid="{6975CB59-F6D5-47D7-9B2B-F1859252D01E}"/>
     <hyperlink ref="I9" r:id="rId13" xr:uid="{51FD74B9-7D50-4F35-A110-D09792590472}"/>
-    <hyperlink ref="J9" r:id="rId14" display="Soft Termination Datasheet" xr:uid="{A87F9D38-C4D0-42C4-A5FD-BA2D180AB2C2}"/>
+    <hyperlink ref="I10" r:id="rId14" xr:uid="{F763EB3C-385C-4BD2-8180-AA365F1A1523}"/>
+    <hyperlink ref="J10" r:id="rId15" display="http://www.infineon.com/dgdl/irf7458pbf.pdf?fileId=5546d462533600a4015355fecb231bfe" xr:uid="{1E53B5FD-77F4-45FD-9FDF-BEE894CA5AA2}"/>
+    <hyperlink ref="J9" r:id="rId16" display="https://search.kemet.com/component-edge/download/datasheet/C0805C104K3RACTU.pdf" xr:uid="{B70F4811-E6D5-48E8-8F0B-CA4BC5243BEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>